<commit_message>
añadidos los csv de las tablas
</commit_message>
<xml_diff>
--- a/Excels/data/2006.xlsx
+++ b/Excels/data/2006.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19900F96-5729-4CA2-98AB-10F77E60FB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796007D7-B281-4AE8-BB91-E4A702DD5A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="871" firstSheet="1" activeTab="9" xr2:uid="{5594292E-C3E6-4C85-A252-B032F651B054}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" tabRatio="871" firstSheet="2" activeTab="9" xr2:uid="{5594292E-C3E6-4C85-A252-B032F651B054}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar" sheetId="2" r:id="rId1"/>
@@ -2883,7 +2883,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D18"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3158,8 +3158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65C4E11-521C-4B4E-AA03-16AC09AD8815}">
   <dimension ref="A1:AA102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="K107" sqref="K107"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3287,9 +3287,6 @@
       <c r="L2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="N2" s="3" t="s">
         <v>149</v>
       </c>
@@ -3297,12 +3294,15 @@
         <v>149</v>
       </c>
       <c r="P2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3343,9 +3343,6 @@
       <c r="L3" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="N3" s="4" t="s">
         <v>147</v>
       </c>
@@ -3353,12 +3350,15 @@
         <v>147</v>
       </c>
       <c r="P3" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3399,22 +3399,22 @@
       <c r="L4" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="N4" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3455,22 +3455,22 @@
       <c r="L5" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="P5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="Q5" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="R5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="S5" s="4" t="s">
         <v>90</v>
       </c>
     </row>
@@ -3511,22 +3511,22 @@
       <c r="L6" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="S6" s="3" t="s">
         <v>146</v>
       </c>
     </row>
@@ -3567,22 +3567,22 @@
       <c r="L7" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="N7" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="P7" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="R7" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="S7" s="4" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3623,22 +3623,22 @@
       <c r="L8" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>90</v>
       </c>
       <c r="Q8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="R8" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="S8" s="3" t="s">
         <v>154</v>
       </c>
     </row>
@@ -3679,22 +3679,22 @@
       <c r="L9" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="P9" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="Q9" s="4" t="s">
         <v>152</v>
       </c>
       <c r="R9" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="S9" s="4" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3729,22 +3729,22 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="N10" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="P10" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="Q10" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="R10" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="S10" s="3" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3785,22 +3785,22 @@
       <c r="L11" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="P11" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="P11" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="Q11" s="4" t="s">
         <v>152</v>
       </c>
       <c r="R11" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="S11" s="4" t="s">
         <v>496</v>
       </c>
     </row>
@@ -3841,22 +3841,22 @@
       <c r="L12" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="N12" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="O12" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="P12" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="Q12" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="R12" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="R12" s="3" t="s">
+      <c r="S12" s="3" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3897,22 +3897,22 @@
       <c r="L13" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="M13" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="N13" s="4" t="s">
         <v>107</v>
       </c>
       <c r="O13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="P13" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="Q13" s="4" t="s">
+      <c r="R13" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="S13" s="4" t="s">
         <v>504</v>
       </c>
     </row>
@@ -3953,20 +3953,20 @@
       <c r="L14" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="N14" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="N14" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="O14" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P14" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3" t="s">
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="R14" s="3" t="s">
+      <c r="S14" s="3" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4007,22 +4007,22 @@
       <c r="L15" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="P15" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="Q15" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="R15" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="S15" s="4" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4059,26 +4059,26 @@
       <c r="L16" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="O16" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P16" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="Q16" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="R16" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="R16" s="3" t="s">
+      <c r="S16" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>558</v>
       </c>
@@ -4115,26 +4115,26 @@
       <c r="L17" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="M17" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="N17" s="4" t="s">
         <v>152</v>
       </c>
       <c r="O17" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="P17" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="P17" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="Q17" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="R17" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="R17" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>323</v>
       </c>
@@ -4171,26 +4171,26 @@
       <c r="L18" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="N18" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="N18" s="3" t="s">
+      <c r="O18" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>153</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>153</v>
       </c>
       <c r="Q18" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="R18" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="R18" s="3" t="s">
+      <c r="S18" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>358</v>
       </c>
@@ -4227,16 +4227,16 @@
       <c r="L19" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="N19" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="4"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>406</v>
       </c>
@@ -4273,24 +4273,24 @@
       <c r="L20" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="N20" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3" t="s">
+      <c r="O20" s="3"/>
+      <c r="P20" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="Q20" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q20" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="R20" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="S20" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>401</v>
       </c>
@@ -4309,26 +4309,26 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="N21" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="O21" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="O21" s="4" t="s">
+      <c r="P21" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="P21" s="4" t="s">
+      <c r="Q21" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="Q21" s="4" t="s">
+      <c r="R21" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="R21" s="4" t="s">
+      <c r="S21" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>342</v>
       </c>
@@ -4365,26 +4365,26 @@
       <c r="L22" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="M22" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="N22" s="3" t="s">
         <v>152</v>
       </c>
       <c r="O22" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P22" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="P22" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="Q22" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="R22" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="R22" s="3" t="s">
+      <c r="S22" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>372</v>
       </c>
@@ -4421,16 +4421,16 @@
       <c r="L23" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4" t="s">
+      <c r="N23" s="4"/>
+      <c r="O23" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="4"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>403</v>
       </c>
@@ -4457,26 +4457,26 @@
       <c r="L24" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="M24" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="N24" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O24" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="O24" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="P24" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q24" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="Q24" s="3" t="s">
+      <c r="R24" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="R24" s="3" t="s">
+      <c r="S24" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>410</v>
       </c>
@@ -4513,26 +4513,26 @@
       <c r="L25" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M25" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="N25" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="O25" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="O25" s="4" t="s">
+      <c r="P25" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="P25" s="4" t="s">
+      <c r="Q25" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="Q25" s="4" t="s">
+      <c r="R25" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="R25" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>415</v>
       </c>
@@ -4567,24 +4567,24 @@
         <v>162</v>
       </c>
       <c r="L26" s="3"/>
-      <c r="M26" s="3" t="s">
+      <c r="N26" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="N26" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="O26" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P26" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="P26" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="Q26" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="R26" s="3"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R26" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="S26" s="3"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>347</v>
       </c>
@@ -4621,18 +4621,18 @@
       <c r="L27" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="M27" s="4" t="s">
+      <c r="N27" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="N27" s="4" t="s">
+      <c r="O27" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="4"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>327</v>
       </c>
@@ -4669,26 +4669,26 @@
       <c r="L28" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="M28" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="N28" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O28" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="O28" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="P28" s="3" t="s">
         <v>152</v>
       </c>
       <c r="Q28" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="R28" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="R28" s="3" t="s">
+      <c r="S28" s="3" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>409</v>
       </c>
@@ -4707,14 +4707,14 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S29" s="4"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>409</v>
       </c>
@@ -4749,26 +4749,26 @@
       <c r="L30" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="M30" s="3" t="s">
+      <c r="N30" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="N30" s="3" t="s">
+      <c r="O30" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="O30" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="P30" s="3" t="s">
-        <v>510</v>
+        <v>152</v>
       </c>
       <c r="Q30" s="3" t="s">
         <v>510</v>
       </c>
       <c r="R30" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="S30" s="3" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>338</v>
       </c>
@@ -4787,14 +4787,14 @@
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S31" s="4"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>338</v>
       </c>
@@ -4815,14 +4815,14 @@
         <v>519</v>
       </c>
       <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" s="3"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>338</v>
       </c>
@@ -4839,22 +4839,22 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="4" t="s">
+      <c r="O33" s="4"/>
+      <c r="P33" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="P33" s="4" t="s">
+      <c r="Q33" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="Q33" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="R33" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="S33" s="4" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>353</v>
       </c>
@@ -4875,18 +4875,18 @@
       <c r="L34" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
-      <c r="Q34" s="3" t="s">
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="R34" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>213</v>
       </c>
@@ -4917,14 +4917,14 @@
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35" s="4"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>345</v>
       </c>
@@ -4959,26 +4959,26 @@
         <v>164</v>
       </c>
       <c r="L36" s="3"/>
-      <c r="M36" s="3" t="s">
+      <c r="N36" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="N36" s="3" t="s">
-        <v>496</v>
       </c>
       <c r="O36" s="3" t="s">
         <v>496</v>
       </c>
       <c r="P36" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="Q36" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="Q36" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="R36" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="S36" s="3" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>386</v>
       </c>
@@ -5013,20 +5013,20 @@
       <c r="L37" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="M37" s="4" t="s">
+      <c r="N37" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
-      <c r="Q37" s="4" t="s">
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="R37" s="4" t="s">
+      <c r="S37" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>400</v>
       </c>
@@ -5063,26 +5063,26 @@
       <c r="L38" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="M38" s="3" t="s">
+      <c r="N38" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="N38" s="3" t="s">
+      <c r="O38" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="O38" s="3" t="s">
+      <c r="P38" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="P38" s="3" t="s">
+      <c r="Q38" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="Q38" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="R38" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="S38" s="3" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>391</v>
       </c>
@@ -5119,26 +5119,26 @@
       <c r="L39" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M39" s="4" t="s">
+      <c r="N39" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="N39" s="4" t="s">
+      <c r="O39" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="O39" s="4" t="s">
+      <c r="P39" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="P39" s="4" t="s">
+      <c r="Q39" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="Q39" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="R39" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="S39" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>396</v>
       </c>
@@ -5175,22 +5175,22 @@
       <c r="L40" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="M40" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="N40" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O40" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="O40" s="3" t="s">
+      <c r="P40" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="P40" s="3" t="s">
+      <c r="Q40" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S40" s="3"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>375</v>
       </c>
@@ -5227,26 +5227,26 @@
       <c r="L41" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="M41" s="4" t="s">
+      <c r="N41" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="N41" s="4" t="s">
+      <c r="O41" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="O41" s="4" t="s">
+      <c r="P41" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="P41" s="4" t="s">
+      <c r="Q41" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="Q41" s="4" t="s">
+      <c r="R41" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="R41" s="4" t="s">
+      <c r="S41" s="4" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>365</v>
       </c>
@@ -5281,20 +5281,20 @@
       <c r="L42" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="M42" s="3" t="s">
+      <c r="N42" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="N42" s="3" t="s">
+      <c r="O42" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="O42" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="P42" s="3"/>
+      <c r="P42" s="3" t="s">
+        <v>152</v>
+      </c>
       <c r="Q42" s="3"/>
       <c r="R42" s="3"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S42" s="3"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>412</v>
       </c>
@@ -5331,26 +5331,26 @@
       <c r="L43" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="M43" s="4" t="s">
+      <c r="N43" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="N43" s="4" t="s">
+      <c r="O43" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="O43" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="P43" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q43" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="Q43" s="4" t="s">
+      <c r="R43" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="R43" s="4" t="s">
+      <c r="S43" s="4" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>367</v>
       </c>
@@ -5387,14 +5387,14 @@
       <c r="L44" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
       <c r="R44" s="3"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S44" s="3"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>340</v>
       </c>
@@ -5415,16 +5415,16 @@
       <c r="L45" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="M45" s="4"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
       <c r="P45" s="4"/>
-      <c r="Q45" s="4" t="s">
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="R45" s="4"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S45" s="4"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>340</v>
       </c>
@@ -5443,14 +5443,14 @@
         <v>527</v>
       </c>
       <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
       <c r="R46" s="3"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S46" s="3"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>405</v>
       </c>
@@ -5487,26 +5487,26 @@
       <c r="L47" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M47" s="4" t="s">
+      <c r="N47" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="N47" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="O47" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="P47" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="P47" s="4" t="s">
+      <c r="Q47" s="4" t="s">
         <v>522</v>
-      </c>
-      <c r="Q47" s="4" t="s">
-        <v>517</v>
       </c>
       <c r="R47" s="4" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S47" s="4" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>331</v>
       </c>
@@ -5541,18 +5541,18 @@
       <c r="L48" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="M48" s="3" t="s">
+      <c r="N48" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="N48" s="3" t="s">
+      <c r="O48" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="O48" s="3"/>
       <c r="P48" s="3"/>
       <c r="Q48" s="3"/>
       <c r="R48" s="3"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S48" s="3"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>369</v>
       </c>
@@ -5569,20 +5569,20 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
-      <c r="P49" s="4" t="s">
-        <v>152</v>
-      </c>
+      <c r="P49" s="4"/>
       <c r="Q49" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="R49" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="R49" s="4" t="s">
+      <c r="S49" s="4" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>362</v>
       </c>
@@ -5601,14 +5601,14 @@
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
       <c r="R50" s="3"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S50" s="3"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>362</v>
       </c>
@@ -5625,24 +5625,24 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4" t="s">
+      <c r="N51" s="4"/>
+      <c r="O51" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="O51" s="4" t="s">
+      <c r="P51" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="P51" s="4" t="s">
+      <c r="Q51" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="Q51" s="4" t="s">
+      <c r="R51" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="R51" s="4" t="s">
+      <c r="S51" s="4" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>477</v>
       </c>
@@ -5661,14 +5661,14 @@
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S52" s="3"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>360</v>
       </c>
@@ -5701,26 +5701,26 @@
       <c r="L53" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M53" s="4" t="s">
+      <c r="N53" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="N53" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="O53" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="P53" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="P53" s="4" t="s">
+      <c r="Q53" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="Q53" s="4" t="s">
+      <c r="R53" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="R53" s="4" t="s">
+      <c r="S53" s="4" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>349</v>
       </c>
@@ -5739,14 +5739,14 @@
         <v>518</v>
       </c>
       <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
       <c r="R54" s="3"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S54" s="3"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>349</v>
       </c>
@@ -5763,22 +5763,22 @@
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="4" t="s">
+      <c r="O55" s="4"/>
+      <c r="P55" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="P55" s="4" t="s">
+      <c r="Q55" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="Q55" s="4" t="s">
+      <c r="R55" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="R55" s="4" t="s">
+      <c r="S55" s="4" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>480</v>
       </c>
@@ -5797,14 +5797,14 @@
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
       <c r="R56" s="3"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S56" s="3"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>460</v>
       </c>
@@ -5829,18 +5829,18 @@
       </c>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
-      <c r="M57" s="4" t="s">
+      <c r="N57" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="N57" s="4"/>
       <c r="O57" s="4"/>
       <c r="P57" s="4"/>
       <c r="Q57" s="4"/>
-      <c r="R57" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R57" s="4"/>
+      <c r="S57" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>373</v>
       </c>
@@ -5859,14 +5859,14 @@
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S58" s="3"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>395</v>
       </c>
@@ -5883,18 +5883,18 @@
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
       <c r="N59" s="4"/>
       <c r="O59" s="4"/>
       <c r="P59" s="4"/>
-      <c r="Q59" s="4" t="s">
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="R59" s="4" t="s">
+      <c r="S59" s="4" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>420</v>
       </c>
@@ -5911,16 +5911,16 @@
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
-      <c r="R60" s="3" t="s">
+      <c r="R60" s="3"/>
+      <c r="S60" s="3" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>464</v>
       </c>
@@ -5937,16 +5937,16 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4" t="s">
+      <c r="N61" s="4"/>
+      <c r="O61" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="O61" s="4"/>
       <c r="P61" s="4"/>
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S61" s="4"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>413</v>
       </c>
@@ -5967,16 +5967,16 @@
       </c>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
-      <c r="M62" s="3" t="s">
+      <c r="N62" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="N62" s="3"/>
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
       <c r="R62" s="3"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S62" s="3"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>426</v>
       </c>
@@ -5993,16 +5993,16 @@
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
-      <c r="P63" s="4" t="s">
+      <c r="P63" s="4"/>
+      <c r="Q63" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S63" s="4"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>336</v>
       </c>
@@ -6019,18 +6019,18 @@
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
-      <c r="P64" s="3" t="s">
-        <v>152</v>
-      </c>
+      <c r="P64" s="3"/>
       <c r="Q64" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="R64" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="R64" s="3"/>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S64" s="3"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>448</v>
       </c>
@@ -6047,18 +6047,18 @@
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
-      <c r="M65" s="4" t="s">
+      <c r="N65" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="N65" s="4"/>
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
-      <c r="Q65" s="4" t="s">
+      <c r="Q65" s="4"/>
+      <c r="R65" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="R65" s="4"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S65" s="4"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>424</v>
       </c>
@@ -6075,16 +6075,16 @@
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
-      <c r="P66" s="3" t="s">
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="Q66" s="3"/>
       <c r="R66" s="3"/>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S66" s="3"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>446</v>
       </c>
@@ -6101,16 +6101,16 @@
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
-      <c r="M67" s="4" t="s">
+      <c r="N67" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="N67" s="4"/>
       <c r="O67" s="4"/>
       <c r="P67" s="4"/>
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S67" s="4"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>443</v>
       </c>
@@ -6129,14 +6129,14 @@
         <v>516</v>
       </c>
       <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
       <c r="Q68" s="3"/>
       <c r="R68" s="3"/>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S68" s="3"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>428</v>
       </c>
@@ -6153,16 +6153,16 @@
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
-      <c r="P69" s="4" t="s">
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S69" s="4"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>473</v>
       </c>
@@ -6181,14 +6181,14 @@
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
-      <c r="M70" s="3"/>
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
       <c r="R70" s="3"/>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S70" s="3"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>457</v>
       </c>
@@ -6207,16 +6207,16 @@
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
       <c r="N71" s="4"/>
       <c r="O71" s="4"/>
       <c r="P71" s="4"/>
       <c r="Q71" s="4"/>
-      <c r="R71" s="4" t="s">
+      <c r="R71" s="4"/>
+      <c r="S71" s="4" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>451</v>
       </c>
@@ -6233,16 +6233,16 @@
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
-      <c r="M72" s="3" t="s">
+      <c r="N72" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="N72" s="3"/>
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
       <c r="Q72" s="3"/>
       <c r="R72" s="3"/>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S72" s="3"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>490</v>
       </c>
@@ -6261,14 +6261,14 @@
       <c r="L73" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="M73" s="4"/>
       <c r="N73" s="4"/>
       <c r="O73" s="4"/>
       <c r="P73" s="4"/>
       <c r="Q73" s="4"/>
       <c r="R73" s="4"/>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S73" s="4"/>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>370</v>
       </c>
@@ -6285,16 +6285,16 @@
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
-      <c r="M74" s="3" t="s">
+      <c r="N74" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="N74" s="3"/>
       <c r="O74" s="3"/>
       <c r="P74" s="3"/>
       <c r="Q74" s="3"/>
       <c r="R74" s="3"/>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S74" s="3"/>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>442</v>
       </c>
@@ -6313,14 +6313,14 @@
         <v>524</v>
       </c>
       <c r="L75" s="4"/>
-      <c r="M75" s="4"/>
       <c r="N75" s="4"/>
       <c r="O75" s="4"/>
       <c r="P75" s="4"/>
       <c r="Q75" s="4"/>
       <c r="R75" s="4"/>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S75" s="4"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>484</v>
       </c>
@@ -6339,14 +6339,14 @@
       </c>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
-      <c r="M76" s="3"/>
       <c r="N76" s="3"/>
       <c r="O76" s="3"/>
       <c r="P76" s="3"/>
       <c r="Q76" s="3"/>
       <c r="R76" s="3"/>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S76" s="3"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>333</v>
       </c>
@@ -6365,14 +6365,14 @@
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
       <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
       <c r="N77" s="4"/>
       <c r="O77" s="4"/>
       <c r="P77" s="4"/>
       <c r="Q77" s="4"/>
       <c r="R77" s="4"/>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S77" s="4"/>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>333</v>
       </c>
@@ -6389,16 +6389,16 @@
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
-      <c r="M78" s="3"/>
       <c r="N78" s="3"/>
       <c r="O78" s="3"/>
       <c r="P78" s="3"/>
       <c r="Q78" s="3"/>
-      <c r="R78" s="3" t="s">
+      <c r="R78" s="3"/>
+      <c r="S78" s="3" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>417</v>
       </c>
@@ -6419,16 +6419,16 @@
       <c r="L79" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M79" s="4"/>
       <c r="N79" s="4"/>
       <c r="O79" s="4"/>
       <c r="P79" s="4"/>
       <c r="Q79" s="4"/>
-      <c r="R79" s="4" t="s">
+      <c r="R79" s="4"/>
+      <c r="S79" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>455</v>
       </c>
@@ -6449,14 +6449,14 @@
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
-      <c r="M80" s="3"/>
       <c r="N80" s="3"/>
       <c r="O80" s="3"/>
       <c r="P80" s="3"/>
       <c r="Q80" s="3"/>
       <c r="R80" s="3"/>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S80" s="3"/>
+    </row>
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>422</v>
       </c>
@@ -6473,16 +6473,16 @@
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
       <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
       <c r="N81" s="4"/>
       <c r="O81" s="4"/>
-      <c r="P81" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="4" t="s">
+        <v>152</v>
+      </c>
       <c r="R81" s="4"/>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S81" s="4"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>436</v>
       </c>
@@ -6499,16 +6499,16 @@
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
-      <c r="M82" s="3"/>
       <c r="N82" s="3"/>
-      <c r="O82" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="P82" s="3"/>
+      <c r="O82" s="3"/>
+      <c r="P82" s="3" t="s">
+        <v>152</v>
+      </c>
       <c r="Q82" s="3"/>
       <c r="R82" s="3"/>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S82" s="3"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>430</v>
       </c>
@@ -6527,14 +6527,14 @@
       <c r="L83" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M83" s="4"/>
       <c r="N83" s="4"/>
       <c r="O83" s="4"/>
       <c r="P83" s="4"/>
       <c r="Q83" s="4"/>
       <c r="R83" s="4"/>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S83" s="4"/>
+    </row>
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>453</v>
       </c>
@@ -6553,14 +6553,14 @@
       <c r="L84" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="M84" s="3"/>
       <c r="N84" s="3"/>
       <c r="O84" s="3"/>
       <c r="P84" s="3"/>
       <c r="Q84" s="3"/>
       <c r="R84" s="3"/>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S84" s="3"/>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>444</v>
       </c>
@@ -6579,14 +6579,14 @@
         <v>152</v>
       </c>
       <c r="L85" s="4"/>
-      <c r="M85" s="4"/>
       <c r="N85" s="4"/>
       <c r="O85" s="4"/>
       <c r="P85" s="4"/>
       <c r="Q85" s="4"/>
       <c r="R85" s="4"/>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S85" s="4"/>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>440</v>
       </c>
@@ -6605,14 +6605,14 @@
         <v>152</v>
       </c>
       <c r="L86" s="3"/>
-      <c r="M86" s="3"/>
       <c r="N86" s="3"/>
       <c r="O86" s="3"/>
       <c r="P86" s="3"/>
       <c r="Q86" s="3"/>
       <c r="R86" s="3"/>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S86" s="3"/>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>482</v>
       </c>
@@ -6631,14 +6631,14 @@
       </c>
       <c r="K87" s="4"/>
       <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
       <c r="N87" s="4"/>
       <c r="O87" s="4"/>
       <c r="P87" s="4"/>
       <c r="Q87" s="4"/>
       <c r="R87" s="4"/>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S87" s="4"/>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>468</v>
       </c>
@@ -6657,14 +6657,14 @@
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
-      <c r="M88" s="3"/>
       <c r="N88" s="3"/>
       <c r="O88" s="3"/>
       <c r="P88" s="3"/>
       <c r="Q88" s="3"/>
       <c r="R88" s="3"/>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S88" s="3"/>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>475</v>
       </c>
@@ -6683,14 +6683,14 @@
       <c r="J89" s="4"/>
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
-      <c r="M89" s="4"/>
       <c r="N89" s="4"/>
       <c r="O89" s="4"/>
       <c r="P89" s="4"/>
       <c r="Q89" s="4"/>
       <c r="R89" s="4"/>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S89" s="4"/>
+    </row>
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>488</v>
       </c>
@@ -6709,14 +6709,14 @@
       <c r="L90" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="M90" s="3"/>
       <c r="N90" s="3"/>
       <c r="O90" s="3"/>
       <c r="P90" s="3"/>
       <c r="Q90" s="3"/>
       <c r="R90" s="3"/>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S90" s="3"/>
+    </row>
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>471</v>
       </c>
@@ -6735,14 +6735,14 @@
       <c r="J91" s="4"/>
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
-      <c r="M91" s="4"/>
       <c r="N91" s="4"/>
       <c r="O91" s="4"/>
       <c r="P91" s="4"/>
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S91" s="4"/>
+    </row>
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>434</v>
       </c>
@@ -6759,16 +6759,16 @@
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
-      <c r="M92" s="3"/>
       <c r="N92" s="3"/>
-      <c r="O92" s="3" t="s">
+      <c r="O92" s="3"/>
+      <c r="P92" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="P92" s="3"/>
       <c r="Q92" s="3"/>
       <c r="R92" s="3"/>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S92" s="3"/>
+    </row>
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>432</v>
       </c>
@@ -6785,16 +6785,16 @@
       <c r="J93" s="4"/>
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
-      <c r="M93" s="4"/>
       <c r="N93" s="4"/>
-      <c r="O93" s="4" t="s">
+      <c r="O93" s="4"/>
+      <c r="P93" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="P93" s="4"/>
       <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S93" s="4"/>
+    </row>
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>438</v>
       </c>
@@ -6811,16 +6811,16 @@
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
-      <c r="M94" s="3"/>
       <c r="N94" s="3"/>
-      <c r="O94" s="3" t="s">
+      <c r="O94" s="3"/>
+      <c r="P94" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="P94" s="3"/>
       <c r="Q94" s="3"/>
       <c r="R94" s="3"/>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S94" s="3"/>
+    </row>
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>408</v>
       </c>
@@ -6839,14 +6839,14 @@
       <c r="J95" s="4"/>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
-      <c r="M95" s="4"/>
       <c r="N95" s="4"/>
       <c r="O95" s="4"/>
       <c r="P95" s="4"/>
       <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S95" s="4"/>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
         <v>556</v>
       </c>
@@ -10625,8 +10625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADDB044-4998-4848-A0BB-5D6E7C903DE0}">
   <dimension ref="A1:T72"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:S72"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="P81" sqref="P81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15019,8 +15019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5687A505-F17C-4A06-9C43-76AF413FFDB1}">
   <dimension ref="A1:AA76"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15148,9 +15148,6 @@
       <c r="L2" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="N2" s="3" t="s">
         <v>149</v>
       </c>
@@ -15158,12 +15155,15 @@
         <v>149</v>
       </c>
       <c r="P2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>151</v>
       </c>
     </row>
@@ -15204,22 +15204,22 @@
       <c r="L3" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="N3" s="4" t="s">
         <v>147</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>151</v>
       </c>
       <c r="Q3" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>150</v>
       </c>
     </row>
@@ -15260,22 +15260,22 @@
       <c r="L4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="N4" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>147</v>
       </c>
       <c r="Q4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="R4" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>149</v>
       </c>
     </row>
@@ -15316,22 +15316,22 @@
       <c r="L5" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="O5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>152</v>
       </c>
     </row>
@@ -15372,22 +15372,22 @@
       <c r="L6" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="R6" s="3" t="s">
+      <c r="S6" s="3" t="s">
         <v>147</v>
       </c>
     </row>
@@ -15428,20 +15428,20 @@
       <c r="L7" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="4"/>
+      <c r="O7" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="O7" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="P7" s="4" t="s">
         <v>152</v>
       </c>
       <c r="Q7" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="R7" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="R7" s="4" t="s">
+      <c r="S7" s="4" t="s">
         <v>161</v>
       </c>
     </row>
@@ -15478,22 +15478,22 @@
       <c r="L8" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="N8" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="O8" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="R8" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="S8" s="3" t="s">
         <v>146</v>
       </c>
     </row>
@@ -15534,22 +15534,22 @@
       <c r="L9" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M9" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="N9" s="4" t="s">
         <v>156</v>
       </c>
       <c r="O9" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="P9" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="Q9" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="R9" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="S9" s="4" t="s">
         <v>156</v>
       </c>
     </row>
@@ -15590,22 +15590,22 @@
       <c r="L10" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="O10" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="P10" s="3" t="s">
         <v>152</v>
       </c>
       <c r="Q10" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="R10" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="S10" s="3" t="s">
         <v>159</v>
       </c>
     </row>
@@ -15646,22 +15646,22 @@
       <c r="L11" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="P11" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="R11" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="R11" s="4" t="s">
+      <c r="S11" s="4" t="s">
         <v>152</v>
       </c>
     </row>
@@ -15702,22 +15702,22 @@
       <c r="L12" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="M12" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="N12" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="P12" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="Q12" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="R12" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R12" s="3" t="s">
+      <c r="S12" s="3" t="s">
         <v>504</v>
       </c>
     </row>
@@ -15758,22 +15758,22 @@
       <c r="L13" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="O13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="P13" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="P13" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="Q13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="R13" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="R13" s="4" t="s">
+      <c r="S13" s="4" t="s">
         <v>160</v>
       </c>
     </row>
@@ -15802,14 +15802,14 @@
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="3" t="s">
+      <c r="N14" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="3" t="s">
+      <c r="R14" s="3"/>
+      <c r="S14" s="3" t="s">
         <v>148</v>
       </c>
     </row>
@@ -15850,22 +15850,22 @@
       <c r="L15" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="M15" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="N15" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="O15" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="O15" s="4" t="s">
+      <c r="P15" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>158</v>
       </c>
       <c r="Q15" s="4" t="s">
         <v>158</v>
       </c>
       <c r="R15" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="S15" s="4" t="s">
         <v>154</v>
       </c>
     </row>
@@ -15904,20 +15904,20 @@
       <c r="L16" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="O16" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P16" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="3"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>221</v>
       </c>
@@ -15954,26 +15954,26 @@
       <c r="L17" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="M17" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="N17" s="4" t="s">
         <v>161</v>
       </c>
       <c r="O17" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="P17" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="P17" s="4" t="s">
+      <c r="Q17" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="Q17" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="R17" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="S17" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>235</v>
       </c>
@@ -16006,26 +16006,26 @@
       <c r="L18" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="N18" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="N18" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="O18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P18" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="P18" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="Q18" s="3" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
       <c r="R18" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>193</v>
       </c>
@@ -16056,14 +16056,14 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="4"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>213</v>
       </c>
@@ -16086,26 +16086,26 @@
       <c r="L20" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="M20" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="N20" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O20" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="O20" s="3" t="s">
+      <c r="P20" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="P20" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="Q20" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>189</v>
       </c>
@@ -16142,26 +16142,26 @@
       <c r="L21" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="M21" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="N21" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="O21" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="O21" s="4" t="s">
+      <c r="P21" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="P21" s="4" t="s">
+      <c r="Q21" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="Q21" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="R21" s="4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>183</v>
       </c>
@@ -16190,26 +16190,26 @@
       <c r="L22" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="M22" s="3" t="s">
+      <c r="N22" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="N22" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="O22" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P22" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>162</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>202</v>
       </c>
@@ -16244,22 +16244,22 @@
       <c r="L23" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="N23" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="O23" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="O23" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="P23" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q23" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="4"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>209</v>
       </c>
@@ -16296,26 +16296,26 @@
       <c r="L24" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="N24" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N24" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="O24" s="3" t="s">
         <v>152</v>
       </c>
       <c r="P24" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q24" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="Q24" s="3" t="s">
+      <c r="R24" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="R24" s="3" t="s">
+      <c r="S24" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>197</v>
       </c>
@@ -16332,20 +16332,20 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
-      <c r="P25" s="4" t="s">
-        <v>152</v>
-      </c>
+      <c r="P25" s="4"/>
       <c r="Q25" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="R25" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="R25" s="4" t="s">
+      <c r="S25" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>311</v>
       </c>
@@ -16362,16 +16362,16 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
-      <c r="P26" s="3" t="s">
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S26" s="3"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>237</v>
       </c>
@@ -16398,14 +16398,14 @@
       <c r="L27" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="4"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>218</v>
       </c>
@@ -16432,26 +16432,26 @@
       <c r="L28" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="N28" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="N28" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="O28" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="P28" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="P28" s="3" t="s">
+      <c r="Q28" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="Q28" s="3" t="s">
+      <c r="R28" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="R28" s="3" t="s">
+      <c r="S28" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>313</v>
       </c>
@@ -16468,16 +16468,16 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
-      <c r="P29" s="4" t="s">
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S29" s="4"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>216</v>
       </c>
@@ -16502,14 +16502,14 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30" s="3"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>216</v>
       </c>
@@ -16536,26 +16536,26 @@
       <c r="L31" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="M31" s="4" t="s">
+      <c r="N31" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="N31" s="4" t="s">
+      <c r="O31" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="O31" s="4" t="s">
+      <c r="P31" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="P31" s="4" t="s">
+      <c r="Q31" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="Q31" s="4" t="s">
+      <c r="R31" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="R31" s="4" t="s">
+      <c r="S31" s="4" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>317</v>
       </c>
@@ -16572,16 +16572,16 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
-      <c r="P32" s="3" t="s">
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" s="3"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>232</v>
       </c>
@@ -16600,26 +16600,26 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="4" t="s">
+      <c r="N33" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="N33" s="4" t="s">
+      <c r="O33" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="O33" s="4" t="s">
+      <c r="P33" s="4" t="s">
         <v>504</v>
-      </c>
-      <c r="P33" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="Q33" s="4" t="s">
         <v>164</v>
       </c>
       <c r="R33" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="S33" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>204</v>
       </c>
@@ -16646,14 +16646,14 @@
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" s="3"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>204</v>
       </c>
@@ -16672,16 +16672,16 @@
         <v>152</v>
       </c>
       <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
-      <c r="R35" s="4" t="s">
+      <c r="R35" s="4"/>
+      <c r="S35" s="4" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>207</v>
       </c>
@@ -16718,26 +16718,26 @@
       <c r="L36" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="M36" s="3" t="s">
+      <c r="N36" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="N36" s="3" t="s">
+      <c r="O36" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="O36" s="3" t="s">
+      <c r="P36" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="P36" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="Q36" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="R36" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="R36" s="3" t="s">
+      <c r="S36" s="3" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>257</v>
       </c>
@@ -16758,16 +16758,16 @@
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
-      <c r="R37" s="4" t="s">
+      <c r="R37" s="4"/>
+      <c r="S37" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>229</v>
       </c>
@@ -16790,14 +16790,14 @@
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S38" s="3"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>261</v>
       </c>
@@ -16816,18 +16816,18 @@
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4" t="s">
+      <c r="N39" s="4"/>
+      <c r="O39" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="O39" s="4"/>
       <c r="P39" s="4"/>
-      <c r="Q39" s="4" t="s">
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="R39" s="4"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S39" s="4"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>277</v>
       </c>
@@ -16846,14 +16846,14 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S40" s="3"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>263</v>
       </c>
@@ -16880,20 +16880,20 @@
       <c r="L41" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="M41" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="N41" s="4"/>
+      <c r="N41" s="4" t="s">
+        <v>152</v>
+      </c>
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="4" t="s">
-        <v>152</v>
-      </c>
+      <c r="Q41" s="4"/>
       <c r="R41" s="4" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S41" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>543</v>
       </c>
@@ -16910,18 +16910,18 @@
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3" t="s">
+      <c r="N42" s="3"/>
+      <c r="O42" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="O42" s="3"/>
       <c r="P42" s="3"/>
-      <c r="Q42" s="3" t="s">
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="R42" s="3"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S42" s="3"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>279</v>
       </c>
@@ -16940,14 +16940,14 @@
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S43" s="4"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>222</v>
       </c>
@@ -16982,26 +16982,26 @@
       <c r="L44" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="M44" s="3" t="s">
+      <c r="N44" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="N44" s="3" t="s">
+      <c r="O44" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="O44" s="3" t="s">
+      <c r="P44" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="P44" s="3" t="s">
+      <c r="Q44" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="Q44" s="3" t="s">
+      <c r="R44" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="R44" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S44" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>181</v>
       </c>
@@ -17026,14 +17026,14 @@
         <v>496</v>
       </c>
       <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S45" s="4"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>181</v>
       </c>
@@ -17052,14 +17052,14 @@
       <c r="L46" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
       <c r="Q46" s="3"/>
       <c r="R46" s="3"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S46" s="3"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>211</v>
       </c>
@@ -17080,14 +17080,14 @@
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
       <c r="P47" s="4"/>
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S47" s="4"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>315</v>
       </c>
@@ -17104,16 +17104,16 @@
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
-      <c r="P48" s="3" t="s">
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="Q48" s="3"/>
       <c r="R48" s="3"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S48" s="3"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>309</v>
       </c>
@@ -17130,16 +17130,16 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="4" t="s">
+      <c r="N49" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="N49" s="4"/>
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S49" s="4"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>205</v>
       </c>
@@ -17158,18 +17158,18 @@
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
-      <c r="Q50" s="3" t="s">
-        <v>152</v>
-      </c>
+      <c r="Q50" s="3"/>
       <c r="R50" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="S50" s="3" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>319</v>
       </c>
@@ -17186,16 +17186,16 @@
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
-      <c r="P51" s="4" t="s">
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S51" s="4"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>288</v>
       </c>
@@ -17214,14 +17214,14 @@
       </c>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S52" s="3"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>544</v>
       </c>
@@ -17240,14 +17240,14 @@
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
       <c r="P53" s="4"/>
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S53" s="4"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>281</v>
       </c>
@@ -17270,14 +17270,14 @@
       <c r="L54" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="M54" s="3"/>
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
       <c r="R54" s="3"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S54" s="3"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>284</v>
       </c>
@@ -17296,14 +17296,14 @@
       </c>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
-      <c r="M55" s="4"/>
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
       <c r="P55" s="4"/>
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S55" s="4"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>275</v>
       </c>
@@ -17322,14 +17322,14 @@
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
       <c r="R56" s="3"/>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S56" s="3"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>301</v>
       </c>
@@ -17348,14 +17348,14 @@
       <c r="L57" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
       <c r="P57" s="4"/>
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S57" s="4"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>286</v>
       </c>
@@ -17374,14 +17374,14 @@
       </c>
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S58" s="3"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>294</v>
       </c>
@@ -17400,18 +17400,18 @@
         <v>152</v>
       </c>
       <c r="L59" s="4"/>
-      <c r="M59" s="4" t="s">
+      <c r="N59" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="N59" s="4"/>
       <c r="O59" s="4"/>
       <c r="P59" s="4"/>
-      <c r="Q59" s="4" t="s">
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="R59" s="4"/>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S59" s="4"/>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>268</v>
       </c>
@@ -17428,16 +17428,16 @@
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
       <c r="Q60" s="3"/>
-      <c r="R60" s="3" t="s">
+      <c r="R60" s="3"/>
+      <c r="S60" s="3" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>255</v>
       </c>
@@ -17454,16 +17454,16 @@
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
-      <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
-      <c r="P61" s="4" t="s">
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S61" s="4"/>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>290</v>
       </c>
@@ -17482,14 +17482,14 @@
       </c>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
       <c r="R62" s="3"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S62" s="3"/>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>546</v>
       </c>
@@ -17506,16 +17506,16 @@
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
       <c r="P63" s="4"/>
-      <c r="Q63" s="4" t="s">
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="R63" s="4"/>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S63" s="4"/>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>305</v>
       </c>
@@ -17532,16 +17532,16 @@
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
-      <c r="M64" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="N64" s="3"/>
+      <c r="N64" s="3" t="s">
+        <v>152</v>
+      </c>
       <c r="O64" s="3"/>
       <c r="P64" s="3"/>
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S64" s="3"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>303</v>
       </c>
@@ -17560,14 +17560,14 @@
       <c r="L65" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M65" s="4"/>
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S65" s="4"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>271</v>
       </c>
@@ -17586,14 +17586,14 @@
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
       <c r="P66" s="3"/>
       <c r="Q66" s="3"/>
       <c r="R66" s="3"/>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S66" s="3"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>307</v>
       </c>
@@ -17610,16 +17610,16 @@
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
-      <c r="M67" s="4" t="s">
+      <c r="N67" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="N67" s="4"/>
       <c r="O67" s="4"/>
       <c r="P67" s="4"/>
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S67" s="4"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>297</v>
       </c>
@@ -17638,14 +17638,14 @@
         <v>520</v>
       </c>
       <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
       <c r="Q68" s="3"/>
       <c r="R68" s="3"/>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S68" s="3"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>299</v>
       </c>
@@ -17664,14 +17664,14 @@
         <v>520</v>
       </c>
       <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
       <c r="P69" s="4"/>
       <c r="Q69" s="4"/>
       <c r="R69" s="4"/>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S69" s="4"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>292</v>
       </c>
@@ -17690,14 +17690,14 @@
       </c>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
-      <c r="M70" s="3"/>
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
       <c r="R70" s="3"/>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S70" s="3"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>272</v>
       </c>
@@ -17716,14 +17716,14 @@
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
       <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
       <c r="N71" s="4"/>
       <c r="O71" s="4"/>
       <c r="P71" s="4"/>
       <c r="Q71" s="4"/>
       <c r="R71" s="4"/>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S71" s="4"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>266</v>
       </c>
@@ -17742,29 +17742,29 @@
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
-      <c r="M72" s="3"/>
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
       <c r="Q72" s="3"/>
       <c r="R72" s="3"/>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S72" s="3"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>557</v>
       </c>

</xml_diff>